<commit_message>
Add updated test results
</commit_message>
<xml_diff>
--- a/random_restart_tests/generations_to_success.xlsx
+++ b/random_restart_tests/generations_to_success.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Khoury Course Scheduling\course-scheduler\io_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Khoury Course Scheduling\course-scheduler\random_restart_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAFA08B-AA74-4EB6-A492-17B751351188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A0FC55-C43D-4440-B0A8-A024D2965628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7440" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{76D46049-9049-48DE-923C-407E73254D16}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{76D46049-9049-48DE-923C-407E73254D16}"/>
   </bookViews>
   <sheets>
     <sheet name="Originals" sheetId="1" r:id="rId1"/>
-    <sheet name="Compare restart and org" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Originals!$A$1:$A$60</definedName>
@@ -62,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="10">
   <si>
     <t>Y</t>
   </si>
@@ -92,18 +91,6 @@
   </si>
   <si>
     <t>Success = 0.999 fitness</t>
-  </si>
-  <si>
-    <t>Attempts</t>
-  </si>
-  <si>
-    <t>Original Iterations</t>
-  </si>
-  <si>
-    <t>Times</t>
-  </si>
-  <si>
-    <t>New Iterations</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45584F05-A657-4744-8957-A8061478DBAD}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -1867,240 +1854,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D71065-5512-43F8-9707-24D7FD3E1F29}">
-  <dimension ref="A1:E26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="16.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.86328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>4347</v>
-      </c>
-      <c r="B2">
-        <v>122.619</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>6924</v>
-      </c>
-      <c r="B3">
-        <v>379.23200000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>1440</v>
-      </c>
-      <c r="B4">
-        <v>25.61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>8377</v>
-      </c>
-      <c r="B5">
-        <v>141.45599999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>6067</v>
-      </c>
-      <c r="B6">
-        <v>356.70499999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>4476</v>
-      </c>
-      <c r="B7">
-        <v>80.263999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>6618</v>
-      </c>
-      <c r="B8">
-        <v>717.03300000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>1903</v>
-      </c>
-      <c r="B9">
-        <v>77.677999999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>3749</v>
-      </c>
-      <c r="B10">
-        <v>109.697</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>1693</v>
-      </c>
-      <c r="B11">
-        <v>30.541</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>251</v>
-      </c>
-      <c r="B12">
-        <v>4.4939999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>9764</v>
-      </c>
-      <c r="B13">
-        <v>161.99799999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>7254</v>
-      </c>
-      <c r="B14">
-        <v>164.96799999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>2494</v>
-      </c>
-      <c r="B15">
-        <v>188.565</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>1666</v>
-      </c>
-      <c r="B16">
-        <v>29.553999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>8640</v>
-      </c>
-      <c r="B17">
-        <v>145.62899999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>5049</v>
-      </c>
-      <c r="B18">
-        <v>90.156999999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>74</v>
-      </c>
-      <c r="B19">
-        <v>1.585</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>3407</v>
-      </c>
-      <c r="B20">
-        <v>127.976</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21">
-        <v>2509</v>
-      </c>
-      <c r="B21">
-        <v>45.783000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22">
-        <v>9366</v>
-      </c>
-      <c r="B22">
-        <v>371.21300000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <v>262</v>
-      </c>
-      <c r="B23">
-        <v>5.04</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>1552</v>
-      </c>
-      <c r="B24">
-        <v>100.88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>3299</v>
-      </c>
-      <c r="B25">
-        <v>59.997999999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>5858</v>
-      </c>
-      <c r="B26">
-        <v>102.11799999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>